<commit_message>
update on interpolating GW elevations
</commit_message>
<xml_diff>
--- a/Topography/LaJara_TopoSurvey/UpReach_LongProfile.xlsx
+++ b/Topography/LaJara_TopoSurvey/UpReach_LongProfile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\Topography\LaJara_TopoSurvey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3441D7A-E82F-4E37-A112-28C25449A781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F2B69E-BB53-459E-9206-E2AF88470AB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{6875A78A-EB74-4CCE-9079-1EDDD22DA4D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2312,8 +2312,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64046064-0207-40E0-86BF-2B34A938C764}">
   <dimension ref="A1:J117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G99" sqref="G99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>